<commit_message>
Fixing Lab 8 charts
</commit_message>
<xml_diff>
--- a/08_baroreceptor_reflex/08_baroreceptor_reflex_data.xlsx
+++ b/08_baroreceptor_reflex/08_baroreceptor_reflex_data.xlsx
@@ -150,7 +150,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -164,73 +164,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -534,7 +481,7 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3:T9"/>
+      <selection activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -590,19 +537,19 @@
       <c r="O2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="5">
         <v>60</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2" s="5">
         <v>80</v>
       </c>
-      <c r="R2" s="2">
+      <c r="R2" s="5">
         <v>100</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="5">
         <v>120</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="5">
         <v>140</v>
       </c>
     </row>
@@ -643,26 +590,26 @@
       <c r="M3" s="4">
         <v>0.74</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3" s="6">
         <f>ABS((B3-I3)/B3)</f>
         <v>1.7391304347826105E-2</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="Q3" s="6">
         <f t="shared" ref="Q3:T3" si="0">ABS((C3-J3)/C3)</f>
         <v>5.2631578947368472E-3</v>
       </c>
-      <c r="R3" s="5">
+      <c r="R3" s="6">
         <f t="shared" si="0"/>
         <v>4.0000000000000036E-2</v>
       </c>
-      <c r="S3" s="5">
+      <c r="S3" s="6">
         <f t="shared" si="0"/>
         <v>5.0000000000000044E-2</v>
       </c>
-      <c r="T3" s="5">
+      <c r="T3" s="6">
         <f t="shared" si="0"/>
         <v>9.5714285714285694</v>
       </c>
@@ -704,26 +651,26 @@
       <c r="M4" s="4">
         <v>5.42</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="P4" s="5">
+      <c r="P4" s="6">
         <f t="shared" ref="P4:P9" si="1">ABS((B4-I4)/B4)</f>
         <v>3.7499999999999895E-2</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="Q4" s="6">
         <f t="shared" ref="Q4:Q9" si="2">ABS((C4-J4)/C4)</f>
         <v>1.5384615384615398E-2</v>
       </c>
-      <c r="R4" s="5">
+      <c r="R4" s="6">
         <f t="shared" ref="R4:R9" si="3">ABS((D4-K4)/D4)</f>
         <v>1.9047619047619063E-2</v>
       </c>
-      <c r="S4" s="5">
+      <c r="S4" s="6">
         <f t="shared" ref="S4:S9" si="4">ABS((E4-L4)/E4)</f>
         <v>2.1428571428571394E-2</v>
       </c>
-      <c r="T4" s="5">
+      <c r="T4" s="6">
         <f t="shared" ref="T4:T9" si="5">ABS((F4-M4)/F4)</f>
         <v>3.7037037037036245E-3</v>
       </c>
@@ -765,26 +712,26 @@
       <c r="M5" s="4">
         <v>52</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="5">
+      <c r="P5" s="6">
         <f t="shared" si="1"/>
         <v>1.1235955056179775E-2</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="Q5" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R5" s="5">
+      <c r="R5" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S5" s="5">
+      <c r="S5" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T5" s="5">
+      <c r="T5" s="6">
         <f t="shared" si="5"/>
         <v>1.9607843137254902E-2</v>
       </c>
@@ -826,26 +773,26 @@
       <c r="M6" s="4">
         <v>76</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="O6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P6" s="5">
+      <c r="P6" s="6">
         <f t="shared" si="1"/>
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="Q6" s="6">
         <f t="shared" si="2"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="R6" s="5">
+      <c r="R6" s="6">
         <f t="shared" si="3"/>
         <v>1.3333333333333334E-2</v>
       </c>
-      <c r="S6" s="5">
+      <c r="S6" s="6">
         <f t="shared" si="4"/>
         <v>4.9382716049382713E-2</v>
       </c>
-      <c r="T6" s="5">
+      <c r="T6" s="6">
         <f t="shared" si="5"/>
         <v>7.3170731707317069E-2</v>
       </c>
@@ -887,26 +834,26 @@
       <c r="M7" s="4">
         <v>3939</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="O7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P7" s="5">
+      <c r="P7" s="6">
         <f t="shared" si="1"/>
         <v>8.2826990725935398E-2</v>
       </c>
-      <c r="Q7" s="5">
+      <c r="Q7" s="6">
         <f t="shared" si="2"/>
         <v>5.6422569027611044E-2</v>
       </c>
-      <c r="R7" s="5">
+      <c r="R7" s="6">
         <f t="shared" si="3"/>
         <v>1.4374881785511632E-2</v>
       </c>
-      <c r="S7" s="5">
+      <c r="S7" s="6">
         <f t="shared" si="4"/>
         <v>4.8323036187113859E-2</v>
       </c>
-      <c r="T7" s="5">
+      <c r="T7" s="6">
         <f t="shared" si="5"/>
         <v>6.9674067076051019E-2</v>
       </c>
@@ -948,26 +895,26 @@
       <c r="M8" s="4">
         <v>1.5299999999999999E-2</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="5">
+      <c r="P8" s="6">
         <f t="shared" si="1"/>
         <v>3.4999999999999962E-2</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="Q8" s="6">
         <f t="shared" si="2"/>
         <v>3.6842105263157857E-2</v>
       </c>
-      <c r="R8" s="5">
+      <c r="R8" s="6">
         <f t="shared" si="3"/>
         <v>3.8888888888888848E-2</v>
       </c>
-      <c r="S8" s="5">
+      <c r="S8" s="6">
         <f t="shared" si="4"/>
         <v>5.2941176470588318E-2</v>
       </c>
-      <c r="T8" s="5">
+      <c r="T8" s="6">
         <f t="shared" si="5"/>
         <v>0.1000000000000001</v>
       </c>
@@ -1009,37 +956,37 @@
       <c r="M9" s="4">
         <v>63.3</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="O9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P9" s="5">
+      <c r="P9" s="6">
         <f t="shared" si="1"/>
         <v>6.8032786885245999E-2</v>
       </c>
-      <c r="Q9" s="5">
+      <c r="Q9" s="6">
         <f t="shared" si="2"/>
         <v>3.1818181818181815E-2</v>
       </c>
-      <c r="R9" s="5">
+      <c r="R9" s="6">
         <f t="shared" si="3"/>
         <v>1.7708333333333364E-2</v>
       </c>
-      <c r="S9" s="5">
+      <c r="S9" s="6">
         <f t="shared" si="4"/>
         <v>7.8205128205128135E-2</v>
       </c>
-      <c r="T9" s="5">
+      <c r="T9" s="6">
         <f t="shared" si="5"/>
         <v>0.12083333333333338</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="P3:T9">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>0.5</formula>
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>